<commit_message>
Update Section 9.1 - Initiative Team - Submission Tool Template.xlsx
</commit_message>
<xml_diff>
--- a/one-cgiar-back/public/templates/Section 9.1 - Initiative Team - Submission Tool Template.xlsx
+++ b/one-cgiar-back/public/templates/Section 9.1 - Initiative Team - Submission Tool Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24603"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar.sharepoint.com/sites/PRMFImplementation/Shared Documents/Online Submissions Tool/6. Full proposal/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_230BC2BC5DEABECAA51BAB55DA7BFC5C23C1546F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{83C6EA03-5E64-49F6-88D5-286671FDAB78}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_230BC2BC5DEABECAA51BAB55DA7BFC5C23C1546F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB8205B1-51DC-45A3-8D58-C2BDCCFF7D8B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="25545" yWindow="-5010" windowWidth="15750" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="25545" yWindow="-5010" windowWidth="15750" windowHeight="12660" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Initiative Team</t>
+  </si>
+  <si>
+    <t>Guidance to complete the initiative team table</t>
+  </si>
   <si>
     <t>Guidance</t>
-  </si>
-  <si>
-    <t>Initiative Team</t>
-  </si>
-  <si>
-    <t>Guidance to complete the initiative team table</t>
   </si>
   <si>
     <t>Where Initiatives anticipate large teams, they may wish to group roles by areas of expertise or by key accountabilities</t>
@@ -125,9 +125,6 @@
     <t>Short description of key  accountabilities </t>
   </si>
   <si>
-    <t>8. Full-Time Equivalent (FTE)</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
@@ -141,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,7 +671,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
@@ -683,35 +680,35 @@
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="7"/>
       <c r="B2" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="7"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="39.75" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -719,7 +716,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="48.75" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="12"/>
       <c r="C5" s="6" t="s">
@@ -728,7 +725,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="51" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="12"/>
       <c r="C6" s="6" t="s">
@@ -737,7 +734,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="57.75" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="12"/>
       <c r="C7" s="6" t="s">
@@ -766,21 +763,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3711579A-A28B-4B5B-A581-2071A766B962}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="25.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -790,29 +786,18 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{B8F468AC-C78E-495B-89D6-3664EDA1941B}">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -837,24 +822,24 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -866,6 +851,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="5ca99b3b-2006-4525-a392-0eea832c2707" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC391CE9C050B2449C4FA40F8913423D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5074f59da554e3220cc55258e77c0ebc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5ca99b3b-2006-4525-a392-0eea832c2707" xmlns:ns3="1dccc405-6d75-4c17-b17b-84e9890663ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ac3b8163f59360d89f4da31268ff34a" ns2:_="" ns3:_="">
     <xsd:import namespace="5ca99b3b-2006-4525-a392-0eea832c2707"/>
@@ -1088,63 +1090,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="5ca99b3b-2006-4525-a392-0eea832c2707" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B123E4B-FEC2-4BBE-9EDC-98934CC4565E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5ca99b3b-2006-4525-a392-0eea832c2707"/>
-    <ds:schemaRef ds:uri="1dccc405-6d75-4c17-b17b-84e9890663ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0238D8B2-E14A-4B21-890D-F93D63658749}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCF9AC-DBD2-44C3-AED6-15E9A2B65DA6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCF9AC-DBD2-44C3-AED6-15E9A2B65DA6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0238D8B2-E14A-4B21-890D-F93D63658749}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="5ca99b3b-2006-4525-a392-0eea832c2707"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1dccc405-6d75-4c17-b17b-84e9890663ca"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B123E4B-FEC2-4BBE-9EDC-98934CC4565E}"/>
 </file>
</xml_diff>